<commit_message>
added paper for hw5
</commit_message>
<xml_diff>
--- a/Lectures/IF5181 Pengenalan Pola/HW5/Recap Papers.xlsx
+++ b/Lectures/IF5181 Pengenalan Pola/HW5/Recap Papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\books\Lectures\IF5181 Pengenalan Pola\HW5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9C8ECEF-82D5-4900-9612-2E4B4D53D90F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A298C041-D671-4B95-8F07-4D3467A9A2A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{2B02FCDE-BE8E-4FD2-9943-36D9391CAFD1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Judul Paper</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>Franz Bellmann, Lea Bunzel, Christoph Demus, Lisa Fellendorf, Olivia Gr ̈aupner,Qiuyi Hu, Tamara Lange, Alica Stuhr, Jian Xi, Dirk Labudde, Michael Spranger</t>
+  </si>
+  <si>
+    <t>Data Processing</t>
+  </si>
+  <si>
+    <t>Klasifikasi buku ke dalam genre berdasarkan blurb dengan jenis klasifikas multilabel</t>
+  </si>
+  <si>
+    <t>Label diencode dengan kode angka. Jika sebuah buku diklasifikasikan ke dalam lebih dari satu kategori, angka representasi kategori tersebut dijumlahkan.</t>
+  </si>
+  <si>
+    <t>Convolutional Neural Networks for Classification of German Blurbs</t>
+  </si>
+  <si>
+    <t>Erdan Genc, Louay Abdelgawad, Viorel Morari, Peter Kluegl</t>
   </si>
 </sst>
 </file>
@@ -93,10 +108,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,10 +430,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCECEC60-4CA5-4CBE-A131-BBDEE869CFBF}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,66 +442,84 @@
     <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.140625" customWidth="1"/>
     <col min="4" max="4" width="35.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:D5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>